<commit_message>
OW, NW, UR, ZG
</commit_message>
<xml_diff>
--- a/ZG_nais_einheiten_unique.xlsx
+++ b/ZG_nais_einheiten_unique.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frehnerm\Documents\excel\Nais LFI\Tabellen Kantone\2019\Vom Kanton Korrigierte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\develops\sensitivewaldstandorteCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025366F3-BDEA-4DEB-B11A-C78DF360EFA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F5DC6B-1A13-4439-82FB-7BDBB0BD5616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vergleich ZG-NaiS" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId2"/>
+    <sheet name="export" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Vergleich ZG-NaiS'!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="112">
   <si>
     <t>7a</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>17ho gelöscht, 45 neu aufgenommen (gibt es auch in NaiS)</t>
+  </si>
+  <si>
+    <t>Bemerkung2</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -452,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -461,13 +464,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -488,9 +488,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -528,9 +528,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -563,26 +563,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,26 +598,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -810,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E94" sqref="A4:E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +805,6 @@
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -859,7 +824,7 @@
       <c r="A5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="7">
         <v>1</v>
       </c>
@@ -868,7 +833,7 @@
       <c r="A6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
@@ -877,7 +842,7 @@
       <c r="A7" s="7">
         <v>2</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="7">
         <v>2</v>
       </c>
@@ -886,7 +851,7 @@
       <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="7" t="s">
         <v>22</v>
       </c>
@@ -895,7 +860,7 @@
       <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="7">
         <v>6</v>
       </c>
@@ -904,7 +869,7 @@
       <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="7" t="s">
         <v>0</v>
       </c>
@@ -913,7 +878,7 @@
       <c r="A11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="7" t="s">
         <v>0</v>
       </c>
@@ -922,7 +887,7 @@
       <c r="A12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="7" t="s">
         <v>1</v>
       </c>
@@ -931,7 +896,7 @@
       <c r="A13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="7" t="s">
         <v>44</v>
       </c>
@@ -940,7 +905,7 @@
       <c r="A14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="7" t="s">
         <v>46</v>
       </c>
@@ -949,7 +914,7 @@
       <c r="A15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="9"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
         <v>48</v>
       </c>
@@ -958,7 +923,7 @@
       <c r="A16" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="7" t="s">
         <v>2</v>
       </c>
@@ -967,7 +932,7 @@
       <c r="A17" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="9"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="7" t="s">
         <v>1</v>
       </c>
@@ -976,7 +941,7 @@
       <c r="A18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="7" t="s">
         <v>50</v>
       </c>
@@ -985,7 +950,7 @@
       <c r="A19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="9"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="7" t="s">
         <v>4</v>
       </c>
@@ -994,7 +959,7 @@
       <c r="A20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="9"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="7" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +968,7 @@
       <c r="A21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="9"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
@@ -1012,7 +977,7 @@
       <c r="A22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="9"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="7" t="s">
         <v>53</v>
       </c>
@@ -1021,7 +986,7 @@
       <c r="A23" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="9"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="7" t="s">
         <v>54</v>
       </c>
@@ -1030,7 +995,7 @@
       <c r="A24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="7" t="s">
         <v>6</v>
       </c>
@@ -1039,7 +1004,7 @@
       <c r="A25" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="9"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="7" t="s">
         <v>56</v>
       </c>
@@ -1048,7 +1013,7 @@
       <c r="A26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="7" t="s">
         <v>58</v>
       </c>
@@ -1057,7 +1022,7 @@
       <c r="A27" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="9"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="7" t="s">
         <v>5</v>
       </c>
@@ -1066,7 +1031,7 @@
       <c r="A28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="9"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="7" t="s">
         <v>12</v>
       </c>
@@ -1075,7 +1040,7 @@
       <c r="A29" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="9"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="7" t="s">
         <v>60</v>
       </c>
@@ -1084,7 +1049,7 @@
       <c r="A30" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="9"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="7" t="s">
         <v>7</v>
       </c>
@@ -1093,7 +1058,7 @@
       <c r="A31" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="7" t="s">
         <v>61</v>
       </c>
@@ -1102,7 +1067,7 @@
       <c r="A32" s="7">
         <v>11</v>
       </c>
-      <c r="B32" s="9"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="7">
         <v>11</v>
       </c>
@@ -1111,7 +1076,7 @@
       <c r="A33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="9"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="7" t="s">
         <v>18</v>
       </c>
@@ -1120,7 +1085,7 @@
       <c r="A34" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="9"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="7" t="s">
         <v>62</v>
       </c>
@@ -1129,7 +1094,7 @@
       <c r="A35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="9"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="7" t="s">
         <v>13</v>
       </c>
@@ -1138,7 +1103,7 @@
       <c r="A36" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="9"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="7" t="s">
         <v>63</v>
       </c>
@@ -1147,7 +1112,7 @@
       <c r="A37" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="9"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="7" t="s">
         <v>19</v>
       </c>
@@ -1156,7 +1121,7 @@
       <c r="A38" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="9"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="7" t="s">
         <v>64</v>
       </c>
@@ -1165,7 +1130,7 @@
       <c r="A39" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="9"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="7" t="s">
         <v>66</v>
       </c>
@@ -1174,7 +1139,7 @@
       <c r="A40" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="9"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="7">
         <v>14</v>
       </c>
@@ -1183,7 +1148,7 @@
       <c r="A41" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="9"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="7">
         <v>14</v>
       </c>
@@ -1192,7 +1157,7 @@
       <c r="A42" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="9"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="7">
         <v>15</v>
       </c>
@@ -1201,7 +1166,7 @@
       <c r="A43" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B43" s="9"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="7">
         <v>15</v>
       </c>
@@ -1210,7 +1175,7 @@
       <c r="A44" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="9"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="7">
         <v>17</v>
       </c>
@@ -1219,7 +1184,7 @@
       <c r="A45" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B45" s="9"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="7">
         <v>18</v>
       </c>
@@ -1228,7 +1193,7 @@
       <c r="A46" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B46" s="9"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="7">
         <v>18</v>
       </c>
@@ -1237,7 +1202,7 @@
       <c r="A47" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="9"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="7" t="s">
         <v>75</v>
       </c>
@@ -1246,7 +1211,7 @@
       <c r="A48" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="9"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="7">
         <v>18</v>
       </c>
@@ -1255,7 +1220,7 @@
       <c r="A49" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B49" s="9"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="7" t="s">
         <v>20</v>
       </c>
@@ -1264,7 +1229,7 @@
       <c r="A50" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="9"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="7" t="s">
         <v>17</v>
       </c>
@@ -1273,7 +1238,7 @@
       <c r="A51" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="9"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="7" t="s">
         <v>80</v>
       </c>
@@ -1282,7 +1247,7 @@
       <c r="A52" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="8" t="s">
         <v>81</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -1293,7 +1258,7 @@
       <c r="A53" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="8" t="s">
         <v>82</v>
       </c>
       <c r="C53" s="7" t="s">
@@ -1304,7 +1269,7 @@
       <c r="A54" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B54" s="9"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="7">
         <v>19</v>
       </c>
@@ -1313,7 +1278,7 @@
       <c r="A55" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B55" s="9"/>
+      <c r="B55" s="8"/>
       <c r="C55" s="7" t="s">
         <v>21</v>
       </c>
@@ -1322,7 +1287,7 @@
       <c r="A56" s="7">
         <v>20</v>
       </c>
-      <c r="B56" s="9"/>
+      <c r="B56" s="8"/>
       <c r="C56" s="7">
         <v>20</v>
       </c>
@@ -1331,7 +1296,7 @@
       <c r="A57" s="7">
         <v>21</v>
       </c>
-      <c r="B57" s="9"/>
+      <c r="B57" s="8"/>
       <c r="C57" s="7">
         <v>21</v>
       </c>
@@ -1340,7 +1305,7 @@
       <c r="A58" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B58" s="9"/>
+      <c r="B58" s="8"/>
       <c r="C58" s="7">
         <v>22</v>
       </c>
@@ -1349,7 +1314,7 @@
       <c r="A59" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="9"/>
+      <c r="B59" s="8"/>
       <c r="C59" s="7" t="s">
         <v>15</v>
       </c>
@@ -1358,7 +1323,7 @@
       <c r="A60" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B60" s="9"/>
+      <c r="B60" s="8"/>
       <c r="C60" s="7" t="s">
         <v>30</v>
       </c>
@@ -1367,7 +1332,7 @@
       <c r="A61" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B61" s="9"/>
+      <c r="B61" s="8"/>
       <c r="C61" s="7">
         <v>26</v>
       </c>
@@ -1376,7 +1341,7 @@
       <c r="A62" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B62" s="9"/>
+      <c r="B62" s="8"/>
       <c r="C62" s="7">
         <v>26</v>
       </c>
@@ -1385,7 +1350,7 @@
       <c r="A63" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B63" s="9"/>
+      <c r="B63" s="8"/>
       <c r="C63" s="7">
         <v>26</v>
       </c>
@@ -1394,7 +1359,7 @@
       <c r="A64" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B64" s="9"/>
+      <c r="B64" s="8"/>
       <c r="C64" s="7">
         <v>26</v>
       </c>
@@ -1403,7 +1368,7 @@
       <c r="A65" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B65" s="9"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="7" t="s">
         <v>23</v>
       </c>
@@ -1412,7 +1377,7 @@
       <c r="A66" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B66" s="9"/>
+      <c r="B66" s="8"/>
       <c r="C66" s="7">
         <v>27</v>
       </c>
@@ -1421,7 +1386,7 @@
       <c r="A67" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B67" s="9"/>
+      <c r="B67" s="8"/>
       <c r="C67" s="7">
         <v>27</v>
       </c>
@@ -1430,7 +1395,7 @@
       <c r="A68" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B68" s="9"/>
+      <c r="B68" s="8"/>
       <c r="C68" s="7">
         <v>27</v>
       </c>
@@ -1445,7 +1410,7 @@
       <c r="A69" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B69" s="9"/>
+      <c r="B69" s="8"/>
       <c r="C69" s="7" t="s">
         <v>9</v>
       </c>
@@ -1454,7 +1419,7 @@
       <c r="A70" s="7">
         <v>28</v>
       </c>
-      <c r="B70" s="9"/>
+      <c r="B70" s="8"/>
       <c r="C70" s="7">
         <v>28</v>
       </c>
@@ -1463,7 +1428,7 @@
       <c r="A71" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B71" s="9"/>
+      <c r="B71" s="8"/>
       <c r="C71" s="7" t="s">
         <v>10</v>
       </c>
@@ -1472,7 +1437,7 @@
       <c r="A72" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B72" s="9"/>
+      <c r="B72" s="8"/>
       <c r="C72" s="7" t="s">
         <v>11</v>
       </c>
@@ -1481,7 +1446,7 @@
       <c r="A73" s="7">
         <v>30</v>
       </c>
-      <c r="B73" s="9"/>
+      <c r="B73" s="8"/>
       <c r="C73" s="7">
         <v>30</v>
       </c>
@@ -1490,7 +1455,7 @@
       <c r="A74" s="7">
         <v>31</v>
       </c>
-      <c r="B74" s="9"/>
+      <c r="B74" s="8"/>
       <c r="C74" s="7">
         <v>31</v>
       </c>
@@ -1499,7 +1464,7 @@
       <c r="A75" s="7">
         <v>32</v>
       </c>
-      <c r="B75" s="9"/>
+      <c r="B75" s="8"/>
       <c r="C75" s="7" t="s">
         <v>98</v>
       </c>
@@ -1508,7 +1473,7 @@
       <c r="A76" s="7">
         <v>43</v>
       </c>
-      <c r="B76" s="9"/>
+      <c r="B76" s="8"/>
       <c r="C76" s="7">
         <v>43</v>
       </c>
@@ -1517,7 +1482,7 @@
       <c r="A77" s="7">
         <v>44</v>
       </c>
-      <c r="B77" s="9"/>
+      <c r="B77" s="8"/>
       <c r="C77" s="7">
         <v>44</v>
       </c>
@@ -1526,7 +1491,7 @@
       <c r="A78" s="7">
         <v>45</v>
       </c>
-      <c r="B78" s="9"/>
+      <c r="B78" s="8"/>
       <c r="C78" s="7">
         <v>45</v>
       </c>
@@ -1535,7 +1500,7 @@
       <c r="A79" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B79" s="9"/>
+      <c r="B79" s="8"/>
       <c r="C79" s="7">
         <v>46</v>
       </c>
@@ -1544,7 +1509,7 @@
       <c r="A80" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B80" s="9"/>
+      <c r="B80" s="8"/>
       <c r="C80" s="7" t="s">
         <v>31</v>
       </c>
@@ -1553,7 +1518,7 @@
       <c r="A81" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B81" s="9"/>
+      <c r="B81" s="8"/>
       <c r="C81" s="7" t="s">
         <v>24</v>
       </c>
@@ -1562,7 +1527,7 @@
       <c r="A82" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B82" s="9"/>
+      <c r="B82" s="8"/>
       <c r="C82" s="7">
         <v>49</v>
       </c>
@@ -1571,7 +1536,7 @@
       <c r="A83" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B83" s="9"/>
+      <c r="B83" s="8"/>
       <c r="C83" s="7">
         <v>50</v>
       </c>
@@ -1580,7 +1545,7 @@
       <c r="A84" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B84" s="9"/>
+      <c r="B84" s="8"/>
       <c r="C84" s="7">
         <v>50</v>
       </c>
@@ -1589,7 +1554,7 @@
       <c r="A85" s="7">
         <v>51</v>
       </c>
-      <c r="B85" s="9"/>
+      <c r="B85" s="8"/>
       <c r="C85" s="7">
         <v>51</v>
       </c>
@@ -1598,7 +1563,7 @@
       <c r="A86" s="7">
         <v>56</v>
       </c>
-      <c r="B86" s="9"/>
+      <c r="B86" s="8"/>
       <c r="C86" s="7">
         <v>56</v>
       </c>
@@ -1607,7 +1572,7 @@
       <c r="A87" s="7">
         <v>57</v>
       </c>
-      <c r="B87" s="9"/>
+      <c r="B87" s="8"/>
       <c r="C87" s="7" t="s">
         <v>32</v>
       </c>
@@ -1616,7 +1581,7 @@
       <c r="A88" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B88" s="9"/>
+      <c r="B88" s="8"/>
       <c r="C88" s="7">
         <v>60</v>
       </c>
@@ -1625,7 +1590,7 @@
       <c r="A89" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B89" s="9" t="s">
+      <c r="B89" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C89" s="7" t="s">
@@ -1636,7 +1601,7 @@
       <c r="A90" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="B90" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C90" s="7" t="s">
@@ -1647,7 +1612,7 @@
       <c r="A91" s="7">
         <v>62</v>
       </c>
-      <c r="B91" s="9"/>
+      <c r="B91" s="8"/>
       <c r="C91" s="7">
         <v>62</v>
       </c>
@@ -1656,7 +1621,7 @@
       <c r="A92" s="7">
         <v>63</v>
       </c>
-      <c r="B92" s="9"/>
+      <c r="B92" s="8"/>
       <c r="C92" s="7">
         <v>67</v>
       </c>
@@ -1665,7 +1630,7 @@
       <c r="A93" s="7">
         <v>71</v>
       </c>
-      <c r="B93" s="9" t="s">
+      <c r="B93" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C93" s="7">
@@ -1676,7 +1641,7 @@
       <c r="A94" s="7">
         <v>71</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C94" s="7" t="s">
@@ -1703,12 +1668,1043 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="7">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>11</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="7">
+        <v>11</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="7">
+        <v>14</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="7">
+        <v>14</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="7">
+        <v>15</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="7">
+        <v>15</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="7">
+        <v>17</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="7">
+        <v>18</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="7">
+        <v>18</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="7">
+        <v>18</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="7">
+        <v>19</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>20</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="7">
+        <v>20</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>21</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="7">
+        <v>21</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="7">
+        <v>22</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="7">
+        <v>26</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="7">
+        <v>26</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="7">
+        <v>26</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="7">
+        <v>26</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B63" s="8"/>
+      <c r="C63" s="7">
+        <v>27</v>
+      </c>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" s="8"/>
+      <c r="C64" s="7">
+        <v>27</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="7">
+        <v>27</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
+        <v>28</v>
+      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="7">
+        <v>28</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
+        <v>30</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="7">
+        <v>30</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <v>31</v>
+      </c>
+      <c r="B71" s="8"/>
+      <c r="C71" s="7">
+        <v>31</v>
+      </c>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
+        <v>32</v>
+      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="7">
+        <v>43</v>
+      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="7">
+        <v>43</v>
+      </c>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
+        <v>44</v>
+      </c>
+      <c r="B74" s="8"/>
+      <c r="C74" s="7">
+        <v>44</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
+        <v>45</v>
+      </c>
+      <c r="B75" s="8"/>
+      <c r="C75" s="7">
+        <v>45</v>
+      </c>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76" s="8"/>
+      <c r="C76" s="7">
+        <v>46</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B77" s="8"/>
+      <c r="C77" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" s="8"/>
+      <c r="C78" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="7">
+        <v>49</v>
+      </c>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" s="8"/>
+      <c r="C80" s="7">
+        <v>50</v>
+      </c>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B81" s="8"/>
+      <c r="C81" s="7">
+        <v>50</v>
+      </c>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="7">
+        <v>51</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="7">
+        <v>51</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
+        <v>56</v>
+      </c>
+      <c r="B83" s="8"/>
+      <c r="C83" s="7">
+        <v>56</v>
+      </c>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="7">
+        <v>57</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="C84" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85" s="8"/>
+      <c r="C85" s="7">
+        <v>60</v>
+      </c>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
+        <v>62</v>
+      </c>
+      <c r="B88" s="8"/>
+      <c r="C88" s="7">
+        <v>62</v>
+      </c>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
+        <v>63</v>
+      </c>
+      <c r="B89" s="8"/>
+      <c r="C89" s="7">
+        <v>67</v>
+      </c>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="7">
+        <v>71</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C90" s="7">
+        <v>71</v>
+      </c>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
+        <v>71</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>